<commit_message>
working through workflowsets for selecting best model spec prior to going bayesian
</commit_message>
<xml_diff>
--- a/example_model_control_stages.xlsx
+++ b/example_model_control_stages.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loren\Documents\R\tidymmm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2CD4ECD-54A5-4CB0-847D-1BDE169D9529}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{281C627F-CE40-4626-9CF8-FACE1FE24781}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{E15138B5-0913-440B-A52B-3172F9D245BA}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="60">
   <si>
     <t>start_name</t>
   </si>
@@ -202,13 +202,16 @@
     <t>Find best seasonality spec?</t>
   </si>
   <si>
-    <t>pick_fft</t>
-  </si>
-  <si>
     <t>seasonality interactions to test?</t>
   </si>
   <si>
     <t>interaction_fft</t>
+  </si>
+  <si>
+    <t>search_seasonality</t>
+  </si>
+  <si>
+    <t>search_randoms</t>
   </si>
 </sst>
 </file>
@@ -570,10 +573,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D79CA1B-8D6F-4588-9F7B-E9E2FAF0425E}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -621,21 +624,21 @@
         <v>55</v>
       </c>
       <c r="B4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B5" t="s">
         <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.5">
@@ -650,24 +653,32 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B7" t="s">
-        <v>53</v>
+      <c r="B7" t="b">
+        <v>0</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A9" t="s">
         <v>51</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>54</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C9" t="s">
         <v>52</v>
       </c>
     </row>

</xml_diff>